<commit_message>
for cycle was replaced by yield from
</commit_message>
<xml_diff>
--- a/atoka/atoka/spiders/output/output.xlsx
+++ b/atoka/atoka/spiders/output/output.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F143"/>
+  <dimension ref="A1:F144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,255 +460,285 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>info@vibramfivefingers.it</t>
+          <t>info@techpro2.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>+39 0331 999777</t>
+          <t>+39 011 007 4111</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>http://www.vibram.com</t>
+          <t>http://www.cnhindustrial.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>sales@vibramfivefingers.it</t>
+          <t>marketing@cnhindustrial.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>+39 0331 999700</t>
+          <t>+39 011 007 4002</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>http://www.us.vibram.com</t>
+          <t>http://www.cnh.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>inquiry@vibram.com</t>
+          <t>reda@techpro2.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>+39 0331 992572</t>
+          <t>+39 011 007 3539</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>http://www.vibram.it</t>
+          <t>http://www.techpro2.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>vibram@vibram.com</t>
+          <t>alessia.domanico@cnhind.com</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>+39 0331 999703</t>
+          <t>+39 011 007 1929</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>http://agriculture.newholland.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>dealerinquiries@vibram.com</t>
+          <t>cristina.formica@cnhind.com</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>+39 335 576 2520</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>hrvusa@vibram.com</t>
+          <t>francesco.polsinelli@cnhind.com</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>+39 335 177 6091</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>rekha.purwaha@vibram.com</t>
+          <t>investor.relations@cnhind.com</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>+39 0731 533111</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>sustainability@vibram.com</t>
+          <t>jorge.gorgen@cnhind.com</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>+39 059 591514</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>uswebsales@vibram.com</t>
+          <t>laura.overall@cnhind.com</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>+39 059 591111</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>"VIBRAM S.P.A."</t>
+          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>00200450120</t>
+          <t>00370290363</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>kumiko.sanada@vibram.jp</t>
+          <t>mediarelations@cnhind.com</t>
         </is>
       </c>
     </row>
@@ -730,17 +760,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>info@techpro2.com</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>+39 011 007 4111</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>http://www.cnhindustrial.com</t>
+          <t>renato.p.fonseca@cnhind.com</t>
         </is>
       </c>
     </row>
@@ -762,17 +782,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>marketing@cnhindustrial.com</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>+39 011 007 4002</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>http://www.cnh.com</t>
+          <t>sustainability@cnhind.com</t>
         </is>
       </c>
     </row>
@@ -794,17 +804,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>reda@techpro2.com</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>+39 011 007 3539</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>http://www.techpro2.com</t>
+          <t>nan.nie@cnhind.com</t>
         </is>
       </c>
     </row>
@@ -826,1853 +826,1863 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>alessia.domanico@cnhind.com</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>+39 011 007 1929</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>http://agriculture.newholland.com</t>
+          <t>rebecca.fabian@cnhind.com</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>cristina.formica@cnhind.com</t>
+          <t>info@filmmaster.com</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>+39 335 576 2520</t>
+          <t>+39 06 692 0501</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>http://www.filmmaster.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>francesco.polsinelli@cnhind.com</t>
+          <t>info@filmmasterevents.com</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>+39 335 177 6091</t>
+          <t>+39 06 545661</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.filmmasterevents.com</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>investor.relations@cnhind.com</t>
+          <t>info@ien-network.com</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>+39 0731 533111</t>
+          <t>+39 06 6992 0563</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>http://www.ien-network.com</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>jorge.gorgen@cnhind.com</t>
+          <t>info@filmmasterproductions.com</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>+39 059 591514</t>
+          <t>+39 06 591 8865</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>http://www.filmmasterproductions.com</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>laura.overall@cnhind.com</t>
+          <t>info@userfarm.com</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>+39 059 591111</t>
+          <t>+39 02 290911</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>mediarelations@cnhind.com</t>
+          <t>info@filmmaster.es</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>renato.p.fonseca@cnhind.com</t>
+          <t>giorgiomarino@filmmaster.com</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>sustainability@cnhind.com</t>
+          <t>press@ien-network.com</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>nan.nie@cnhind.com</t>
+          <t>job@filmmasterproductions.com</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CNH INDUSTRIAL ITALIA S.P.A.</t>
+          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>00370290363</t>
+          <t>06008721000</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>rebecca.fabian@cnhind.com</t>
+          <t>incontra@civita.it</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BALDINI + CASTOLDI S.R.L.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>info@baldinicastoldi.it</t>
+          <t>info@vibramfivefingers.it</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>+39 02 9455 9601</t>
+          <t>+39 0331 999777</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>http://www.baldinicastoldi.it</t>
+          <t>http://www.vibram.com</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BALDINI + CASTOLDI S.R.L.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>amministrazione@baldinicastoldi.it</t>
+          <t>sales@vibramfivefingers.it</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>+39 02 9455 9621</t>
+          <t>+39 0331 999700</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>http://www.us.vibram.com</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BALDINI + CASTOLDI S.R.L.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>shop@baldinicastoldi.it</t>
+          <t>inquiry@vibram.com</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>+39 02 9455 9608</t>
+          <t>+39 0331 992572</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>http://www.vibram.it</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BALDINI + CASTOLDI S.R.L.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>manoscritti@baldinicastoldi.it</t>
+          <t>vibram@vibram.com</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>+39 0331 999703</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BALDINI + CASTOLDI S.R.L.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>rights@baldinicastoldi.it</t>
+          <t>dealerinquiries@vibram.com</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BALDINI + CASTOLDI S.R.L.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>g.civiletti@baldinicastoldi.it</t>
+          <t>hrvusa@vibram.com</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BALDINI + CASTOLDI S.R.L.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>08218010968</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>social@baldinicastoldi.it</t>
+          <t>rekha.purwaha@vibram.com</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>info@filmmaster.com</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>+39 06 692 0501</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>http://www.filmmaster.com</t>
+          <t>sustainability@vibram.com</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>info@filmmasterevents.com</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>+39 06 545661</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>https://www.filmmasterevents.com</t>
+          <t>uswebsales@vibram.com</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>"VIBRAM S.P.A."</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>00200450120</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>info@ien-network.com</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>+39 06 6992 0563</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>http://www.ien-network.com</t>
+          <t>kumiko.sanada@vibram.jp</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>info@filmmasterproductions.com</t>
+          <t>info@bmg.com</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>+39 06 591 8865</t>
+          <t>+39 02 7767 7300</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>http://www.filmmasterproductions.com</t>
+          <t>http://www.bmg.com</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>info@userfarm.com</t>
+          <t>info@bmgtalpamusic.com</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>+39 02 290911</t>
+          <t>+49 30 300133300</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>info@filmmaster.es</t>
+          <t>info.cn@bmg.com</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>+39 02 9188 3080</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>giorgiomarino@filmmaster.com</t>
+          <t>info.es@bmg.com</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>+39 02 7767 7390</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>press@ien-network.com</t>
+          <t>info.fr@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>job@filmmasterproductions.com</t>
+          <t>info.it@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ITALIAN ENTERTAINMENT NETWORK SOCIETA' PER AZIONI IN FORMA ABBREVIATA I.E.N. S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>06008721000</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>incontra@civita.it</t>
+          <t>info.se@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>info@edidomus.it</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>+39 02 824721</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>http://www.edidomus.it</t>
+          <t>info.uk@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>info@domusweb.it</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>+39 02 8247 2529</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>http://www.domusweb.it</t>
+          <t>info.us@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>amministrazione@edidomus.it</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>+39 02 8247 2385</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>http://pubblicitaonline.edidomus.it</t>
+          <t>licensing@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>direttore@domusweb.it</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>+39 02 8247 2253</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>http://abbonati.shoped.it</t>
+          <t>news@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>sales@edidomus.it</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>+39 02 5656 8800</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>http://www.dueruote.it</t>
+          <t>info.au@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>06702050961</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>assistenza@edidomus.it</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>+39 02 8920 0810</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>http://www.quattroruote.it</t>
+          <t>jodie.feld@bmg.com</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>servizioclienti@edidomus.it</t>
+          <t>info@manetti.com</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>+39 02 8247 2418</t>
+          <t>+39 055 436261</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>http://www.manetti.com</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>webmaster@edidomus.it</t>
+          <t>marketing@manetti.com</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>+39 02 8247 2386</t>
+          <t>+39 055 436 2615</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>http://www.goldchef.shop</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>pubblicita@edidomus.it</t>
+          <t>marketing@manetti.it</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>+39 02 8247 2383</t>
+          <t>+39 055 436 2614</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>responsabiledati@edidomus.it</t>
+          <t>commerciale@manetti.com</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>+39 055 436 2613</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>rights@edidomus.it</t>
+          <t>admin@manetti.it</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>+39 055 436 2611</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>ufficiostampa@edidomus.it</t>
+          <t>goldleaf@manetti.it</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>+39 055 352817</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>assistenzabenidigitali@edidomus.it</t>
+          <t>goldchef@manetti.it</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>+39 055 330954</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>07835550158</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>info.auto@edidomus.it</t>
+          <t>00389280488</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>+39 055 330953</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>07835550158</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>subscriptions@edidomus.it</t>
+          <t>00389280488</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>+39 055 330952</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>07835550158</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>uf.abbonamenti@edidomus.it</t>
+          <t>00389280488</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>+39 055 321 8294</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>07835550158</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>uf.vendite@edidomus.it</t>
+          <t>00389280488</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>+39 055 321 8086</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>07835550158</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>redazione@domusweb.it</t>
+          <t>00389280488</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>+39 055 321 8085</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>EDITORIALE DOMUS S.P.A.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>07835550158</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>07835550158</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>redazione@dueruote.it</t>
+          <t>00389280488</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>+39 055 321 8084</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>06702050961</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>info@bmg.com</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>+39 02 7767 7300</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>http://www.bmg.com</t>
+          <t>+39 055 321 8083</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>06702050961</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>info@bmgtalpamusic.com</t>
+          <t>00389280488</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>+49 30 300133300</t>
+          <t>+39 055 321 7489</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>info.cn@bmg.com</t>
+          <t>info@edidomus.it</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>+39 02 9188 3080</t>
+          <t>+39 02 824721</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>http://www.edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>info.es@bmg.com</t>
+          <t>info@domusweb.it</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>+39 02 7767 7390</t>
+          <t>+39 02 8247 2529</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>http://www.domusweb.it</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>info.fr@bmg.com</t>
+          <t>amministrazione@edidomus.it</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>+39 02 8247 2385</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>http://pubblicitaonline.edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>info.it@bmg.com</t>
+          <t>direttore@domusweb.it</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>+39 02 8247 2253</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>http://abbonati.shoped.it</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>info.se@bmg.com</t>
+          <t>sales@edidomus.it</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>+39 02 5656 8800</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>http://www.dueruote.it</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>info.uk@bmg.com</t>
+          <t>assistenza@edidomus.it</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>+39 02 8920 0810</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>http://www.quattroruote.it</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>info.us@bmg.com</t>
+          <t>servizioclienti@edidomus.it</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>+39 02 8247 2418</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>licensing@bmg.com</t>
+          <t>webmaster@edidomus.it</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>+39 02 8247 2386</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>news@bmg.com</t>
+          <t>pubblicita@edidomus.it</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>+39 02 8247 2383</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>info.au@bmg.com</t>
+          <t>responsabiledati@edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>BMG RIGHTS MANAGEMENT (ITALY) S.R.L.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>06702050961</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>jodie.feld@bmg.com</t>
+          <t>rights@edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>info@manetti.com</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>+39 055 436261</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>http://www.manetti.com</t>
+          <t>ufficiostampa@edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>marketing@manetti.com</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>+39 055 436 2615</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>http://www.goldchef.shop</t>
+          <t>assistenzabenidigitali@edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>marketing@manetti.it</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>+39 055 436 2614</t>
+          <t>info.auto@edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>commerciale@manetti.com</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>+39 055 436 2611</t>
+          <t>subscriptions@edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>admin@manetti.it</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>+39 055 352817</t>
+          <t>uf.abbonamenti@edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>goldleaf@manetti.it</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>+39 055 330954</t>
+          <t>uf.vendite@edidomus.it</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>00389280488</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>+39 055 330953</t>
+          <t>07835550158</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>redazione@domusweb.it</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>EDITORIALE DOMUS S.P.A.</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>07835550158</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>00389280488</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>+39 055 330952</t>
+          <t>07835550158</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>redazione@dueruote.it</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>01711850154</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>01711850154</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>webmaster@genialloyd.it</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>+39 055 321 8294</t>
+          <t>+39 02 2835</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>http://www.genialloyd.it</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>01711850154</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>01711850154</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>alessandra.valentini@genialloyd.it</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>+39 055 321 8086</t>
+          <t>+39 02 2805 2805</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>01711850154</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>00389280488</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>+39 055 321 8085</t>
+          <t>01711850154</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>dpo.genialloyd@genialloyd.it</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>01711850154</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>00389280488</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>+39 055 321 8084</t>
+          <t>01711850154</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>dpo@genialloyd.it</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>01711850154</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>00389280488</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>+39 055 321 8083</t>
+          <t>01711850154</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>privacy@genialloyd.it</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>GIUSTO MANETTI BATTILORO S.P.A.</t>
+          <t>ENI S.P.A.</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>00484960588</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>00389280488</t>
+          <t>00905811006</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>info@eniscuola.net</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>+39 055 321 7489</t>
+          <t>+39 06 59881</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>http://www.eni.com</t>
         </is>
       </c>
     </row>
@@ -2694,17 +2704,17 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>info@eniscuola.net</t>
+          <t>postmaster@eni.it</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>+39 06 59881</t>
+          <t>+39 06 59821</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>http://www.eni.com</t>
+          <t>http://www.eniscuola.net</t>
         </is>
       </c>
     </row>
@@ -2726,17 +2736,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>postmaster@eni.it</t>
+          <t>agenzia.centrocards@eni.com</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>+39 06 59821</t>
+          <t>+39 06 5982 4210</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>http://www.eniscuola.net</t>
+          <t>http://report.eni.com</t>
         </is>
       </c>
     </row>
@@ -2758,17 +2768,17 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>agenzia.centrocards@eni.com</t>
+          <t>agenzia.centronordcards@eni.com</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>+39 06 5982 4210</t>
+          <t>+39 06 5982 2645</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>http://report.eni.com</t>
+          <t>http://www.enistation.com</t>
         </is>
       </c>
     </row>
@@ -2790,17 +2800,17 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>agenzia.centronordcards@eni.com</t>
+          <t>agenzia.centrosudcards@eni.com</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>+39 06 5982 2645</t>
+          <t>+39 06 5982 2030</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>http://www.enistation.com</t>
+          <t>http://eni-learning.com</t>
         </is>
       </c>
     </row>
@@ -2822,17 +2832,17 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>agenzia.centrosudcards@eni.com</t>
+          <t>agenzia.nordestcards@eni.com</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>+39 06 5982 2030</t>
+          <t>+39 06 5078 0283</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>http://eni-learning.com</t>
+          <t>http://multicard.eni.com</t>
         </is>
       </c>
     </row>
@@ -2854,17 +2864,17 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>agenzia.nordestcards@eni.com</t>
+          <t>agenzia.nordovestcards@eni.com</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>+39 06 5078 0283</t>
+          <t>+39 02 930 7367</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>http://multicard.eni.com</t>
+          <t>http://oilproducts.eni.com</t>
         </is>
       </c>
     </row>
@@ -2886,17 +2896,17 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>agenzia.nordovestcards@eni.com</t>
+          <t>agenzia.sudcards@eni.com</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>+39 02 930 7367</t>
+          <t>+39 02 5205 1651</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>http://oilproducts.eni.com</t>
+          <t>http://eprocurement.eni.it</t>
         </is>
       </c>
     </row>
@@ -2918,17 +2928,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>agenzia.sudcards@eni.com</t>
+          <t>alessandro.torello@eni.com</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>+39 02 5205 1651</t>
+          <t>+39 0183 293283</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>http://eprocurement.eni.it</t>
+          <t>http://test-ecatalog.eni.it</t>
         </is>
       </c>
     </row>
@@ -2950,17 +2960,17 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>alessandro.torello@eni.com</t>
+          <t>archivio.storico@eni.com</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>+39 0183 293283</t>
+          <t>+39 0161 392020</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>http://test-ecatalog.eni.it</t>
+          <t>http://www.eventi-eni.it</t>
         </is>
       </c>
     </row>
@@ -2982,17 +2992,17 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>archivio.storico@eni.com</t>
+          <t>blocco.cartemulticard@eni.com</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>+39 0161 392020</t>
+          <t>+39 0143 686556</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>http://www.eventi-eni.it</t>
+          <t>http://www.schoolnet.eni.it</t>
         </is>
       </c>
     </row>
@@ -3014,17 +3024,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>blocco.cartemulticard@eni.com</t>
+          <t>bolzoni_investor@eni.com</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>+39 0143 686556</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>http://www.schoolnet.eni.it</t>
+          <t>+39 0143 686245</t>
         </is>
       </c>
     </row>
@@ -3046,12 +3051,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>bolzoni_investor@eni.com</t>
+          <t>bristot_investor@eni.com</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>+39 0143 686245</t>
+          <t>+39 0131 972049</t>
         </is>
       </c>
     </row>
@@ -3073,12 +3078,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>bristot_investor@eni.com</t>
+          <t>centroservizi.multicard@eni.com</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>+39 0131 972049</t>
+          <t>+39 0131 52409</t>
         </is>
       </c>
     </row>
@@ -3100,12 +3105,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>centroservizi.multicard@eni.com</t>
+          <t>customercare.enistation@eni.com</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>+39 0131 52409</t>
+          <t>+39 011 98201</t>
         </is>
       </c>
     </row>
@@ -3127,12 +3132,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>customercare.enistation@eni.com</t>
+          <t>ebusiness.support@eni.com</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>+39 011 98201</t>
+          <t>+39 011 923 5678</t>
         </is>
       </c>
     </row>
@@ -3154,12 +3159,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>ebusiness.support@eni.com</t>
+          <t>eirlib.selezione@eni.com</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>+39 011 923 5678</t>
+          <t>+39 011 652 2511</t>
         </is>
       </c>
     </row>
@@ -3181,12 +3186,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>eirlib.selezione@eni.com</t>
+          <t>enifoundation@eni.com</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>+39 011 652 2511</t>
+          <t>+39 010 714307</t>
         </is>
       </c>
     </row>
@@ -3208,12 +3213,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>enifoundation@eni.com</t>
+          <t>erika.mandraffino@eni.com</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>+39 010 714307</t>
+          <t>+39 010 5771</t>
         </is>
       </c>
     </row>
@@ -3235,12 +3240,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>erika.mandraffino@eni.com</t>
+          <t>filippo.cotalini@eni.com</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>+39 010 5771</t>
+          <t>+39 010 29181</t>
         </is>
       </c>
     </row>
@@ -3262,12 +3267,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>filippo.cotalini@eni.com</t>
-        </is>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>+39 010 29181</t>
+          <t>info.scuolamattei@eni.com</t>
         </is>
       </c>
     </row>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>info.scuolamattei@eni.com</t>
+          <t>info.wuerzburg@eni.com</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>info.wuerzburg@eni.com</t>
+          <t>infobenelux@eni.com</t>
         </is>
       </c>
     </row>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>infobenelux@eni.com</t>
+          <t>investor.relations@eni.com</t>
         </is>
       </c>
     </row>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>investor.relations@eni.com</t>
+          <t>liu_investor@eni.com</t>
         </is>
       </c>
     </row>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>liu_investor@eni.com</t>
+          <t>lubesapac@eni.com</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>lubesapac@eni.com</t>
+          <t>maestridigitali@eni.com</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>maestridigitali@eni.com</t>
+          <t>marmorato_investor@eni.com</t>
         </is>
       </c>
     </row>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>marmorato_investor@eni.com</t>
+          <t>procartes.fr@eni.com</t>
         </is>
       </c>
     </row>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>procartes.fr@eni.com</t>
+          <t>quaggia_investor@eni.com</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>quaggia_investor@eni.com</t>
+          <t>request@eni.com</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>request@eni.com</t>
+          <t>roberto.albini@eni.com</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>roberto.albini@eni.com</t>
+          <t>sahota_investor@eni.com</t>
         </is>
       </c>
     </row>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>sahota_investor@eni.com</t>
+          <t>salesbenelux@eni.com</t>
         </is>
       </c>
     </row>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>salesbenelux@eni.com</t>
+          <t>segreteriasocietaria.azionisti@eni.com</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>segreteriasocietaria.azionisti@eni.com</t>
+          <t>sostenibilita@eni.com</t>
         </is>
       </c>
     </row>
@@ -3619,7 +3619,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>sostenibilita@eni.com</t>
+          <t>sperotto_investor@eni.com</t>
         </is>
       </c>
     </row>
@@ -3641,7 +3641,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>sperotto_investor@eni.com</t>
+          <t>ufficio.stampa@eni.com</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>ufficio.stampa@eni.com</t>
+          <t>verkoopbenelux@eni.com</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>verkoopbenelux@eni.com</t>
+          <t>opensourcecommerc@eni.it</t>
         </is>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>opensourcecommerc@eni.it</t>
+          <t>cardservice@eniaustria.at</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>cardservice@eniaustria.at</t>
+          <t>eni.france@enifrance.fr</t>
         </is>
       </c>
     </row>
@@ -3751,186 +3751,181 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>eni.france@enifrance.fr</t>
+          <t>sarnataro_universita@enicorporateuniversity.eni.it</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>ENI S.P.A.</t>
+          <t>BALDINI + CASTOLDI S.R.L.</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>00484960588</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>00905811006</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>sarnataro_universita@enicorporateuniversity.eni.it</t>
+          <t>info@baldinicastoldi.it</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>+39 02 9455 9601</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>http://www.baldinicastoldi.it</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
+          <t>BALDINI + CASTOLDI S.R.L.</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>webmaster@genialloyd.it</t>
+          <t>amministrazione@baldinicastoldi.it</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>+39 02 2835</t>
-        </is>
-      </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>http://www.genialloyd.it</t>
+          <t>+39 02 9455 9621</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
+          <t>BALDINI + CASTOLDI S.R.L.</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>alessandra.valentini@genialloyd.it</t>
+          <t>shop@baldinicastoldi.it</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>+39 02 2805 2805</t>
+          <t>+39 02 9455 9608</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
+          <t>BALDINI + CASTOLDI S.R.L.</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>dpo.genialloyd@genialloyd.it</t>
+          <t>manoscritti@baldinicastoldi.it</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
+          <t>BALDINI + CASTOLDI S.R.L.</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>dpo@genialloyd.it</t>
+          <t>rights@baldinicastoldi.it</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>GENIALLOYD SOCIETA' PER AZIONI DI ASSICURAZIONI S.P.A. O IN FORMA ABBREVIATA, GENIALLOYD S.P.A.</t>
+          <t>BALDINI + CASTOLDI S.R.L.</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>01711850154</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>privacy@genialloyd.it</t>
+          <t>g.civiletti@baldinicastoldi.it</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>IL SOLE 24 ORE S.P.A.</t>
+          <t>BALDINI + CASTOLDI S.R.L.</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>00777910159</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>00777910159</t>
+          <t>08218010968</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>info@24orecultura.com</t>
-        </is>
-      </c>
-      <c r="E137" t="inlineStr">
-        <is>
-          <t>+39 02 4677 6814</t>
-        </is>
-      </c>
-      <c r="F137" t="inlineStr">
-        <is>
-          <t>http://www.gruppo24ore.ilsole24ore.com</t>
+          <t>social@baldinicastoldi.it</t>
         </is>
       </c>
     </row>
@@ -3952,17 +3947,17 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>ginevra.cozzi@ilsole24ore.com</t>
+          <t>info@24orecultura.com</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>+39 02 30221</t>
+          <t>+39 02 4677 6814</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>http://www.casa24.ilsole24ore.com</t>
+          <t>http://www.gruppo24ore.ilsole24ore.com</t>
         </is>
       </c>
     </row>
@@ -3984,17 +3979,17 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>investor.relations@ilsole24ore.com</t>
+          <t>ginevra.cozzi@ilsole24ore.com</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>+39 02 063 0221</t>
+          <t>+39 02 30221</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>http://www.ilsole24ore.com</t>
+          <t>http://www.casa24.ilsole24ore.com</t>
         </is>
       </c>
     </row>
@@ -4016,17 +4011,17 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>ilsole24ore@pecserviziotitoli.it</t>
+          <t>investor.relations@ilsole24ore.com</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>+39 0863 9051</t>
+          <t>+39 02 063 0221</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>http://www.gruppo.ilsole24ore.com</t>
+          <t>http://www.ilsole24ore.com</t>
         </is>
       </c>
     </row>
@@ -4048,17 +4043,17 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>letterealsole@sole24ore.com</t>
+          <t>ilsole24ore@pecserviziotitoli.it</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>+39 06 5422 5580</t>
+          <t>+39 0863 9051</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>http://www.24orecultura.com</t>
+          <t>http://www.gruppo.ilsole24ore.com</t>
         </is>
       </c>
     </row>
@@ -4080,17 +4075,17 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>privacy@info.ilsole24ore.com</t>
+          <t>letterealsole@sole24ore.com</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>+39 06 30221</t>
+          <t>+39 06 5422 5580</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>http://multimedia.b2b24.it</t>
+          <t>http://www.24orecultura.com</t>
         </is>
       </c>
     </row>
@@ -4112,10 +4107,42 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
+          <t>privacy@info.ilsole24ore.com</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>+39 06 30221</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>http://multimedia.b2b24.it</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>IL SOLE 24 ORE S.P.A.</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>00777910159</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>00777910159</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
           <t>ufficiomilano@pecserviziotitoli.it</t>
         </is>
       </c>
-      <c r="E143" t="inlineStr">
+      <c r="E144" t="inlineStr">
         <is>
           <t>+39 02 4677 6850</t>
         </is>

</xml_diff>